<commit_message>
changed gui to run the data manipulation when selecting an excel file
</commit_message>
<xml_diff>
--- a/cucc.xlsx
+++ b/cucc.xlsx
@@ -1,23 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25831"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://myoffice.accenture.com/personal/b_toth_accenture_com/Documents/Documents/vsc/JavaToExcel/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="46" documentId="11_EE941C785640BC5A4E1AD874663862C597D57206" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{66662013-123F-4231-BF0C-CD57FA8F41D6}"/>
   <bookViews>
-    <workbookView xWindow="1500" yWindow="1500" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1500" yWindow="1500" windowWidth="17280" windowHeight="8970"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <calcPr calcId="124519"/>
+  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -36,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="11">
   <si>
     <t>Rendszám</t>
   </si>
@@ -74,8 +68,9 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -139,7 +134,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normál" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -197,7 +192,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -232,7 +227,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -416,20 +411,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B14"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:B34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="15.5546875" customWidth="1"/>
-    <col min="2" max="2" width="10.21875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="15.5703125"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="10.28515625"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -437,112 +432,283 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2">
       <c r="A2" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B2">
         <f>COUNTIF(A:A,A2) - 1</f>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
       <c r="A4" t="s">
         <v>2</v>
       </c>
       <c r="B4">
         <f>COUNTIF(A:A,A4) - COUNTIF(A2,A4)</f>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
       <c r="A5" t="s">
         <v>3</v>
       </c>
       <c r="B5">
         <f>COUNTIF(A:A,A5) - COUNTIF(A2,A5)</f>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
       <c r="A6" t="s">
         <v>2</v>
       </c>
       <c r="B6">
         <f>(COUNTIF(A:A,A6)-COUNTIF(A2,A6))</f>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
       <c r="A7" t="s">
         <v>3</v>
       </c>
       <c r="B7">
         <f>(COUNTIF(A:A,A7)-COUNTIF(A2,A7))</f>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
       <c r="A8" t="s">
         <v>4</v>
       </c>
       <c r="B8">
         <f>(COUNTIF(A:A,A8)-COUNTIF(A2,A8))</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
       <c r="A9" t="s">
         <v>5</v>
       </c>
       <c r="B9">
         <f>(COUNTIF(A:A,A9)-COUNTIF(A2,A9))</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
       <c r="A10" t="s">
         <v>6</v>
       </c>
       <c r="B10">
         <f>(COUNTIF(A:A,A10)-COUNTIF(A2,A10))</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
       <c r="A11" t="s">
         <v>7</v>
       </c>
       <c r="B11">
         <f>(COUNTIF(A:A,A11)-COUNTIF(A2,A11))</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
       <c r="A12" t="s">
         <v>8</v>
       </c>
       <c r="B12">
         <f>(COUNTIF(A:A,A12)-COUNTIF(A2,A12))</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
       <c r="A13" t="s">
         <v>9</v>
       </c>
       <c r="B13">
         <f>(COUNTIF(A:A,A13)-COUNTIF(A2,A13))</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
       <c r="A14" t="s">
         <v>10</v>
       </c>
       <c r="B14">
         <f>(COUNTIF(A:A,A14)-COUNTIF(A2,A14))</f>
-        <v>1</v>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2">
+      <c r="A15" t="s">
+        <v>2</v>
+      </c>
+      <c r="B15">
+        <f>(COUNTIF(A:A,A15)-COUNTIF(A2,A15))</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2">
+      <c r="A16" t="s">
+        <v>3</v>
+      </c>
+      <c r="B16">
+        <f>(COUNTIF(A:A,A16)-COUNTIF(A2,A16))</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B17">
+        <f>(COUNTIF(A:A,A17)-COUNTIF(A2,A17))</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18" t="s">
+        <v>3</v>
+      </c>
+      <c r="B18">
+        <f>(COUNTIF(A:A,A18)-COUNTIF(A2,A18))</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19" t="s">
+        <v>4</v>
+      </c>
+      <c r="B19">
+        <f>(COUNTIF(A:A,A19)-COUNTIF(A2,A19))</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2">
+      <c r="A20" t="s">
+        <v>5</v>
+      </c>
+      <c r="B20">
+        <f>(COUNTIF(A:A,A20)-COUNTIF(A2,A20))</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2">
+      <c r="A21" t="s">
+        <v>6</v>
+      </c>
+      <c r="B21">
+        <f>(COUNTIF(A:A,A21)-COUNTIF(A2,A21))</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2">
+      <c r="A22" t="s">
+        <v>7</v>
+      </c>
+      <c r="B22">
+        <f>(COUNTIF(A:A,A22)-COUNTIF(A2,A22))</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2">
+      <c r="A23" t="s">
+        <v>8</v>
+      </c>
+      <c r="B23">
+        <f>(COUNTIF(A:A,A23)-COUNTIF(A2,A23))</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2">
+      <c r="A24" t="s">
+        <v>9</v>
+      </c>
+      <c r="B24">
+        <f>(COUNTIF(A:A,A24)-COUNTIF(A2,A24))</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2">
+      <c r="A25" t="s">
+        <v>10</v>
+      </c>
+      <c r="B25">
+        <f>(COUNTIF(A:A,A25)-COUNTIF(A2,A25))</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="s">
+        <v>2</v>
+      </c>
+      <c r="B26">
+        <f>(COUNTIF(A:A,A26)-COUNTIF(A2,A26))</f>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="s">
+        <v>3</v>
+      </c>
+      <c r="B27">
+        <f>(COUNTIF(A:A,A27)-COUNTIF(A2,A27))</f>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="s">
+        <v>4</v>
+      </c>
+      <c r="B28">
+        <f>(COUNTIF(A:A,A28)-COUNTIF(A2,A28))</f>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="s">
+        <v>5</v>
+      </c>
+      <c r="B29">
+        <f>(COUNTIF(A:A,A29)-COUNTIF(A2,A29))</f>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="s">
+        <v>6</v>
+      </c>
+      <c r="B30">
+        <f>(COUNTIF(A:A,A30)-COUNTIF(A2,A30))</f>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="s">
+        <v>7</v>
+      </c>
+      <c r="B31">
+        <f>(COUNTIF(A:A,A31)-COUNTIF(A2,A31))</f>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="s">
+        <v>8</v>
+      </c>
+      <c r="B32">
+        <f>(COUNTIF(A:A,A32)-COUNTIF(A2,A32))</f>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="s">
+        <v>9</v>
+      </c>
+      <c r="B33">
+        <f>(COUNTIF(A:A,A33)-COUNTIF(A2,A33))</f>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="s">
+        <v>10</v>
+      </c>
+      <c r="B34">
+        <f>(COUNTIF(A:A,A34)-COUNTIF(A2,A34))</f>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
refractoring the sheet fuctionality: now the user can pick between all available sheets instead of manually writing the sheetname
</commit_message>
<xml_diff>
--- a/cucc.xlsx
+++ b/cucc.xlsx
@@ -8,6 +8,7 @@
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Munka1" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="true"/>
   <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="11">
   <si>
     <t>Rendszám</t>
   </si>
@@ -412,7 +413,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B70"/>
+  <dimension ref="A1:B97"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
@@ -438,7 +439,7 @@
       </c>
       <c r="B2">
         <f>COUNTIF(A:A,A2) - 1</f>
-        <v>4</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -447,7 +448,7 @@
       </c>
       <c r="B4">
         <f>COUNTIF(A:A,A4) - COUNTIF(A2,A4)</f>
-        <v>4</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -456,7 +457,7 @@
       </c>
       <c r="B5">
         <f>COUNTIF(A:A,A5) - COUNTIF(A2,A5)</f>
-        <v>4</v>
+        <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -465,7 +466,7 @@
       </c>
       <c r="B6">
         <f>(COUNTIF(A:A,A6)-COUNTIF(A2,A6))</f>
-        <v>4</v>
+        <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -474,7 +475,7 @@
       </c>
       <c r="B7">
         <f>(COUNTIF(A:A,A7)-COUNTIF(A2,A7))</f>
-        <v>4</v>
+        <v>9</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -483,7 +484,7 @@
       </c>
       <c r="B8">
         <f>(COUNTIF(A:A,A8)-COUNTIF(A2,A8))</f>
-        <v>2</v>
+        <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -492,7 +493,7 @@
       </c>
       <c r="B9">
         <f>(COUNTIF(A:A,A9)-COUNTIF(A2,A9))</f>
-        <v>2</v>
+        <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -501,7 +502,7 @@
       </c>
       <c r="B10">
         <f>(COUNTIF(A:A,A10)-COUNTIF(A2,A10))</f>
-        <v>2</v>
+        <v>7</v>
       </c>
     </row>
     <row r="11" spans="1:2">
@@ -510,7 +511,7 @@
       </c>
       <c r="B11">
         <f>(COUNTIF(A:A,A11)-COUNTIF(A2,A11))</f>
-        <v>2</v>
+        <v>7</v>
       </c>
     </row>
     <row r="12" spans="1:2">
@@ -519,7 +520,7 @@
       </c>
       <c r="B12">
         <f>(COUNTIF(A:A,A12)-COUNTIF(A2,A12))</f>
-        <v>2</v>
+        <v>7</v>
       </c>
     </row>
     <row r="13" spans="1:2">
@@ -528,7 +529,7 @@
       </c>
       <c r="B13">
         <f>(COUNTIF(A:A,A13)-COUNTIF(A2,A13))</f>
-        <v>2</v>
+        <v>7</v>
       </c>
     </row>
     <row r="14" spans="1:2">
@@ -537,7 +538,7 @@
       </c>
       <c r="B14">
         <f>(COUNTIF(A:A,A14)-COUNTIF(A2,A14))</f>
-        <v>2</v>
+        <v>7</v>
       </c>
     </row>
     <row r="15" spans="1:2">
@@ -546,7 +547,7 @@
       </c>
       <c r="B15">
         <f>(COUNTIF(A:A,A15)-COUNTIF(A2,A15))</f>
-        <v>4</v>
+        <v>9</v>
       </c>
     </row>
     <row r="16" spans="1:2">
@@ -555,7 +556,7 @@
       </c>
       <c r="B16">
         <f>(COUNTIF(A:A,A16)-COUNTIF(A2,A16))</f>
-        <v>4</v>
+        <v>9</v>
       </c>
     </row>
     <row r="17" spans="1:2">
@@ -564,7 +565,7 @@
       </c>
       <c r="B17">
         <f>(COUNTIF(A:A,A17)-COUNTIF(A2,A17))</f>
-        <v>4</v>
+        <v>9</v>
       </c>
     </row>
     <row r="18" spans="1:2">
@@ -573,7 +574,7 @@
       </c>
       <c r="B18">
         <f>(COUNTIF(A:A,A18)-COUNTIF(A2,A18))</f>
-        <v>4</v>
+        <v>9</v>
       </c>
     </row>
     <row r="19" spans="1:2">
@@ -582,7 +583,7 @@
       </c>
       <c r="B19">
         <f>(COUNTIF(A:A,A19)-COUNTIF(A2,A19))</f>
-        <v>2</v>
+        <v>7</v>
       </c>
     </row>
     <row r="20" spans="1:2">
@@ -591,7 +592,7 @@
       </c>
       <c r="B20">
         <f>(COUNTIF(A:A,A20)-COUNTIF(A2,A20))</f>
-        <v>2</v>
+        <v>7</v>
       </c>
     </row>
     <row r="21" spans="1:2">
@@ -600,7 +601,7 @@
       </c>
       <c r="B21">
         <f>(COUNTIF(A:A,A21)-COUNTIF(A2,A21))</f>
-        <v>2</v>
+        <v>7</v>
       </c>
     </row>
     <row r="22" spans="1:2">
@@ -609,7 +610,7 @@
       </c>
       <c r="B22">
         <f>(COUNTIF(A:A,A22)-COUNTIF(A2,A22))</f>
-        <v>2</v>
+        <v>7</v>
       </c>
     </row>
     <row r="23" spans="1:2">
@@ -618,7 +619,7 @@
       </c>
       <c r="B23">
         <f>(COUNTIF(A:A,A23)-COUNTIF(A2,A23))</f>
-        <v>2</v>
+        <v>7</v>
       </c>
     </row>
     <row r="24" spans="1:2">
@@ -627,7 +628,7 @@
       </c>
       <c r="B24">
         <f>(COUNTIF(A:A,A24)-COUNTIF(A2,A24))</f>
-        <v>2</v>
+        <v>7</v>
       </c>
     </row>
     <row r="25" spans="1:2">
@@ -636,371 +637,644 @@
       </c>
       <c r="B25">
         <f>(COUNTIF(A:A,A25)-COUNTIF(A2,A25))</f>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="26">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2">
       <c r="A26" t="s">
         <v>2</v>
       </c>
       <c r="B26">
         <f>(COUNTIF(A:A,A26)-COUNTIF(A2,A26))</f>
-      </c>
-    </row>
-    <row r="27">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2">
       <c r="A27" t="s">
         <v>3</v>
       </c>
       <c r="B27">
         <f>(COUNTIF(A:A,A27)-COUNTIF(A2,A27))</f>
-      </c>
-    </row>
-    <row r="28">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2">
       <c r="A28" t="s">
         <v>4</v>
       </c>
       <c r="B28">
         <f>(COUNTIF(A:A,A28)-COUNTIF(A2,A28))</f>
-      </c>
-    </row>
-    <row r="29">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2">
       <c r="A29" t="s">
         <v>5</v>
       </c>
       <c r="B29">
         <f>(COUNTIF(A:A,A29)-COUNTIF(A2,A29))</f>
-      </c>
-    </row>
-    <row r="30">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2">
       <c r="A30" t="s">
         <v>6</v>
       </c>
       <c r="B30">
         <f>(COUNTIF(A:A,A30)-COUNTIF(A2,A30))</f>
-      </c>
-    </row>
-    <row r="31">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2">
       <c r="A31" t="s">
         <v>7</v>
       </c>
       <c r="B31">
         <f>(COUNTIF(A:A,A31)-COUNTIF(A2,A31))</f>
-      </c>
-    </row>
-    <row r="32">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2">
       <c r="A32" t="s">
         <v>8</v>
       </c>
       <c r="B32">
         <f>(COUNTIF(A:A,A32)-COUNTIF(A2,A32))</f>
-      </c>
-    </row>
-    <row r="33">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2">
       <c r="A33" t="s">
         <v>9</v>
       </c>
       <c r="B33">
         <f>(COUNTIF(A:A,A33)-COUNTIF(A2,A33))</f>
-      </c>
-    </row>
-    <row r="34">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2">
       <c r="A34" t="s">
         <v>10</v>
       </c>
       <c r="B34">
         <f>(COUNTIF(A:A,A34)-COUNTIF(A2,A34))</f>
-      </c>
-    </row>
-    <row r="35">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2">
       <c r="A35" t="s">
         <v>2</v>
       </c>
       <c r="B35">
         <f>(COUNTIF(A:A,A35)-COUNTIF(A2,A35))</f>
-      </c>
-    </row>
-    <row r="36">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2">
       <c r="A36" t="s">
         <v>3</v>
       </c>
       <c r="B36">
         <f>(COUNTIF(A:A,A36)-COUNTIF(A2,A36))</f>
-      </c>
-    </row>
-    <row r="37">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2">
       <c r="A37" t="s">
         <v>4</v>
       </c>
       <c r="B37">
         <f>(COUNTIF(A:A,A37)-COUNTIF(A2,A37))</f>
-      </c>
-    </row>
-    <row r="38">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2">
       <c r="A38" t="s">
         <v>5</v>
       </c>
       <c r="B38">
         <f>(COUNTIF(A:A,A38)-COUNTIF(A2,A38))</f>
-      </c>
-    </row>
-    <row r="39">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2">
       <c r="A39" t="s">
         <v>6</v>
       </c>
       <c r="B39">
         <f>(COUNTIF(A:A,A39)-COUNTIF(A2,A39))</f>
-      </c>
-    </row>
-    <row r="40">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2">
       <c r="A40" t="s">
         <v>7</v>
       </c>
       <c r="B40">
         <f>(COUNTIF(A:A,A40)-COUNTIF(A2,A40))</f>
-      </c>
-    </row>
-    <row r="41">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2">
       <c r="A41" t="s">
         <v>8</v>
       </c>
       <c r="B41">
         <f>(COUNTIF(A:A,A41)-COUNTIF(A2,A41))</f>
-      </c>
-    </row>
-    <row r="42">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2">
       <c r="A42" t="s">
         <v>9</v>
       </c>
       <c r="B42">
         <f>(COUNTIF(A:A,A42)-COUNTIF(A2,A42))</f>
-      </c>
-    </row>
-    <row r="43">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2">
       <c r="A43" t="s">
         <v>10</v>
       </c>
       <c r="B43">
         <f>(COUNTIF(A:A,A43)-COUNTIF(A2,A43))</f>
-      </c>
-    </row>
-    <row r="44">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2">
       <c r="A44" t="s">
         <v>2</v>
       </c>
       <c r="B44">
         <f>(COUNTIF(A:A,A44)-COUNTIF(A2,A44))</f>
-      </c>
-    </row>
-    <row r="45">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2">
       <c r="A45" t="s">
         <v>3</v>
       </c>
       <c r="B45">
         <f>(COUNTIF(A:A,A45)-COUNTIF(A2,A45))</f>
-      </c>
-    </row>
-    <row r="46">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2">
       <c r="A46" t="s">
         <v>4</v>
       </c>
       <c r="B46">
         <f>(COUNTIF(A:A,A46)-COUNTIF(A2,A46))</f>
-      </c>
-    </row>
-    <row r="47">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2">
       <c r="A47" t="s">
         <v>5</v>
       </c>
       <c r="B47">
         <f>(COUNTIF(A:A,A47)-COUNTIF(A2,A47))</f>
-      </c>
-    </row>
-    <row r="48">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2">
       <c r="A48" t="s">
         <v>6</v>
       </c>
       <c r="B48">
         <f>(COUNTIF(A:A,A48)-COUNTIF(A2,A48))</f>
-      </c>
-    </row>
-    <row r="49">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2">
       <c r="A49" t="s">
         <v>7</v>
       </c>
       <c r="B49">
         <f>(COUNTIF(A:A,A49)-COUNTIF(A2,A49))</f>
-      </c>
-    </row>
-    <row r="50">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2">
       <c r="A50" t="s">
         <v>8</v>
       </c>
       <c r="B50">
         <f>(COUNTIF(A:A,A50)-COUNTIF(A2,A50))</f>
-      </c>
-    </row>
-    <row r="51">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2">
       <c r="A51" t="s">
         <v>9</v>
       </c>
       <c r="B51">
         <f>(COUNTIF(A:A,A51)-COUNTIF(A2,A51))</f>
-      </c>
-    </row>
-    <row r="52">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2">
       <c r="A52" t="s">
         <v>10</v>
       </c>
       <c r="B52">
         <f>(COUNTIF(A:A,A52)-COUNTIF(A2,A52))</f>
-      </c>
-    </row>
-    <row r="53">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2">
       <c r="A53" t="s">
         <v>2</v>
       </c>
       <c r="B53">
         <f>(COUNTIF(A:A,A53)-COUNTIF(A2,A53))</f>
-      </c>
-    </row>
-    <row r="54">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2">
       <c r="A54" t="s">
         <v>3</v>
       </c>
       <c r="B54">
         <f>(COUNTIF(A:A,A54)-COUNTIF(A2,A54))</f>
-      </c>
-    </row>
-    <row r="55">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2">
       <c r="A55" t="s">
         <v>4</v>
       </c>
       <c r="B55">
         <f>(COUNTIF(A:A,A55)-COUNTIF(A2,A55))</f>
-      </c>
-    </row>
-    <row r="56">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2">
       <c r="A56" t="s">
         <v>5</v>
       </c>
       <c r="B56">
         <f>(COUNTIF(A:A,A56)-COUNTIF(A2,A56))</f>
-      </c>
-    </row>
-    <row r="57">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2">
       <c r="A57" t="s">
         <v>6</v>
       </c>
       <c r="B57">
         <f>(COUNTIF(A:A,A57)-COUNTIF(A2,A57))</f>
-      </c>
-    </row>
-    <row r="58">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2">
       <c r="A58" t="s">
         <v>7</v>
       </c>
       <c r="B58">
         <f>(COUNTIF(A:A,A58)-COUNTIF(A2,A58))</f>
-      </c>
-    </row>
-    <row r="59">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2">
       <c r="A59" t="s">
         <v>8</v>
       </c>
       <c r="B59">
         <f>(COUNTIF(A:A,A59)-COUNTIF(A2,A59))</f>
-      </c>
-    </row>
-    <row r="60">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2">
       <c r="A60" t="s">
         <v>9</v>
       </c>
       <c r="B60">
         <f>(COUNTIF(A:A,A60)-COUNTIF(A2,A60))</f>
-      </c>
-    </row>
-    <row r="61">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2">
       <c r="A61" t="s">
         <v>10</v>
       </c>
       <c r="B61">
         <f>(COUNTIF(A:A,A61)-COUNTIF(A2,A61))</f>
-      </c>
-    </row>
-    <row r="62">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2">
       <c r="A62" t="s">
         <v>2</v>
       </c>
       <c r="B62">
         <f>(COUNTIF(A:A,A62)-COUNTIF(A2,A62))</f>
-      </c>
-    </row>
-    <row r="63">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2">
       <c r="A63" t="s">
         <v>3</v>
       </c>
       <c r="B63">
         <f>(COUNTIF(A:A,A63)-COUNTIF(A2,A63))</f>
-      </c>
-    </row>
-    <row r="64">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2">
       <c r="A64" t="s">
         <v>4</v>
       </c>
       <c r="B64">
         <f>(COUNTIF(A:A,A64)-COUNTIF(A2,A64))</f>
-      </c>
-    </row>
-    <row r="65">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2">
       <c r="A65" t="s">
         <v>5</v>
       </c>
       <c r="B65">
         <f>(COUNTIF(A:A,A65)-COUNTIF(A2,A65))</f>
-      </c>
-    </row>
-    <row r="66">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2">
       <c r="A66" t="s">
         <v>6</v>
       </c>
       <c r="B66">
         <f>(COUNTIF(A:A,A66)-COUNTIF(A2,A66))</f>
-      </c>
-    </row>
-    <row r="67">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2">
       <c r="A67" t="s">
         <v>7</v>
       </c>
       <c r="B67">
         <f>(COUNTIF(A:A,A67)-COUNTIF(A2,A67))</f>
-      </c>
-    </row>
-    <row r="68">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2">
       <c r="A68" t="s">
         <v>8</v>
       </c>
       <c r="B68">
         <f>(COUNTIF(A:A,A68)-COUNTIF(A2,A68))</f>
-      </c>
-    </row>
-    <row r="69">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2">
       <c r="A69" t="s">
         <v>9</v>
       </c>
       <c r="B69">
         <f>(COUNTIF(A:A,A69)-COUNTIF(A2,A69))</f>
-      </c>
-    </row>
-    <row r="70">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2">
       <c r="A70" t="s">
         <v>10</v>
       </c>
       <c r="B70">
         <f>(COUNTIF(A:A,A70)-COUNTIF(A2,A70))</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="s">
+        <v>2</v>
+      </c>
+      <c r="B71">
+        <f>(COUNTIF(A:A,A71)-COUNTIF(A2,A71))</f>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="s">
+        <v>3</v>
+      </c>
+      <c r="B72">
+        <f>(COUNTIF(A:A,A72)-COUNTIF(A2,A72))</f>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="s">
+        <v>4</v>
+      </c>
+      <c r="B73">
+        <f>(COUNTIF(A:A,A73)-COUNTIF(A2,A73))</f>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="s">
+        <v>5</v>
+      </c>
+      <c r="B74">
+        <f>(COUNTIF(A:A,A74)-COUNTIF(A2,A74))</f>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="s">
+        <v>6</v>
+      </c>
+      <c r="B75">
+        <f>(COUNTIF(A:A,A75)-COUNTIF(A2,A75))</f>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="s">
+        <v>7</v>
+      </c>
+      <c r="B76">
+        <f>(COUNTIF(A:A,A76)-COUNTIF(A2,A76))</f>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="s">
+        <v>8</v>
+      </c>
+      <c r="B77">
+        <f>(COUNTIF(A:A,A77)-COUNTIF(A2,A77))</f>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="s">
+        <v>9</v>
+      </c>
+      <c r="B78">
+        <f>(COUNTIF(A:A,A78)-COUNTIF(A2,A78))</f>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="s">
+        <v>10</v>
+      </c>
+      <c r="B79">
+        <f>(COUNTIF(A:A,A79)-COUNTIF(A2,A79))</f>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="s">
+        <v>2</v>
+      </c>
+      <c r="B80">
+        <f>(COUNTIF(A:A,A80)-COUNTIF(A2,A80))</f>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="s">
+        <v>3</v>
+      </c>
+      <c r="B81">
+        <f>(COUNTIF(A:A,A81)-COUNTIF(A2,A81))</f>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="s">
+        <v>4</v>
+      </c>
+      <c r="B82">
+        <f>(COUNTIF(A:A,A82)-COUNTIF(A2,A82))</f>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="s">
+        <v>5</v>
+      </c>
+      <c r="B83">
+        <f>(COUNTIF(A:A,A83)-COUNTIF(A2,A83))</f>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="s">
+        <v>6</v>
+      </c>
+      <c r="B84">
+        <f>(COUNTIF(A:A,A84)-COUNTIF(A2,A84))</f>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="s">
+        <v>7</v>
+      </c>
+      <c r="B85">
+        <f>(COUNTIF(A:A,A85)-COUNTIF(A2,A85))</f>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="s">
+        <v>8</v>
+      </c>
+      <c r="B86">
+        <f>(COUNTIF(A:A,A86)-COUNTIF(A2,A86))</f>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="s">
+        <v>9</v>
+      </c>
+      <c r="B87">
+        <f>(COUNTIF(A:A,A87)-COUNTIF(A2,A87))</f>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="s">
+        <v>10</v>
+      </c>
+      <c r="B88">
+        <f>(COUNTIF(A:A,A88)-COUNTIF(A2,A88))</f>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="s">
+        <v>2</v>
+      </c>
+      <c r="B89">
+        <f>(COUNTIF(A:A,A89)-COUNTIF(A2,A89))</f>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="s">
+        <v>3</v>
+      </c>
+      <c r="B90">
+        <f>(COUNTIF(A:A,A90)-COUNTIF(A2,A90))</f>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="s">
+        <v>4</v>
+      </c>
+      <c r="B91">
+        <f>(COUNTIF(A:A,A91)-COUNTIF(A2,A91))</f>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="s">
+        <v>5</v>
+      </c>
+      <c r="B92">
+        <f>(COUNTIF(A:A,A92)-COUNTIF(A2,A92))</f>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="s">
+        <v>6</v>
+      </c>
+      <c r="B93">
+        <f>(COUNTIF(A:A,A93)-COUNTIF(A2,A93))</f>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="s">
+        <v>7</v>
+      </c>
+      <c r="B94">
+        <f>(COUNTIF(A:A,A94)-COUNTIF(A2,A94))</f>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="s">
+        <v>8</v>
+      </c>
+      <c r="B95">
+        <f>(COUNTIF(A:A,A95)-COUNTIF(A2,A95))</f>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="s">
+        <v>9</v>
+      </c>
+      <c r="B96">
+        <f>(COUNTIF(A:A,A96)-COUNTIF(A2,A96))</f>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="s">
+        <v>10</v>
+      </c>
+      <c r="B97">
+        <f>(COUNTIF(A:A,A97)-COUNTIF(A2,A97))</f>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
added new button, so the user can manually insert the LicensePlates + manually calculate the frequency of them.
</commit_message>
<xml_diff>
--- a/cucc.xlsx
+++ b/cucc.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="16">
   <si>
     <t xml:space="preserve">Rendszám</t>
   </si>
@@ -29,34 +29,46 @@
     <t xml:space="preserve">Gyakoriság</t>
   </si>
   <si>
+    <t xml:space="preserve">CCC-111</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ABC-120</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ABC-121</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ABC-122</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ABC-123</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ABC-124</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ABC-125</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ABC-126</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ABC-127</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ABC-128</t>
+  </si>
+  <si>
     <t xml:space="preserve">BBB-567</t>
   </si>
   <si>
-    <t xml:space="preserve">ABC-120</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ABC-121</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ABC-122</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ABC-123</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ABC-124</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ABC-125</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ABC-126</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ABC-127</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ABC-128</t>
+    <t xml:space="preserve">BBB-111</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BBB-123</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BBB-112</t>
   </si>
 </sst>
 </file>
@@ -247,15 +259,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B107"/>
+  <dimension ref="A1:B112"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A106" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C113" activeCellId="0" sqref="C113"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="15.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="10.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="10.29"/>
   </cols>
   <sheetData>
@@ -276,6 +288,7 @@
         <v>1</v>
       </c>
     </row>
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
         <v>3</v>
@@ -1205,10 +1218,55 @@
     </row>
     <row r="107" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A107" s="1" t="s">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="B107" s="1" t="n">
         <f aca="false">(COUNTIF(A:A,A107)-COUNTIF(A2,A107))</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="108" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A108" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B108" s="1" t="n">
+        <f aca="false">(COUNTIF(A:A,A108)-COUNTIF(A2,A108))</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="109" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A109" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B109" s="1" t="n">
+        <f aca="false">(COUNTIF(A:A,A109)-COUNTIF(A2,A109))</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="110" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A110" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B110" s="1" t="n">
+        <f aca="false">(COUNTIF(A:A,A110)-COUNTIF(A2,A110))</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="111" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A111" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B111" s="1" t="n">
+        <f aca="false">(COUNTIF(A:A,A111)-COUNTIF(A2,A111))</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="112" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A112" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B112" s="1" t="n">
+        <f aca="false">(COUNTIF(A:A,A112)-COUNTIF(A2,A112))</f>
         <v>1</v>
       </c>
     </row>

</xml_diff>